<commit_message>
Started refactoring of document requesting
 * to do: stemming of requested words
 * to do: download of document is corrupted
 * to do: removing old code stuff
</commit_message>
<xml_diff>
--- a/ui/src/test/resources/exampledocs/TestTabelle.xlsx
+++ b/ui/src/test/resources/exampledocs/TestTabelle.xlsx
@@ -4,41 +4,57 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Übersicht" sheetId="1" r:id="rId1"/>
+    <sheet name="Probe 1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="11">
+  <si>
+    <t>Fabian Mauz</t>
+  </si>
   <si>
     <t>Probennummer</t>
   </si>
   <si>
-    <t>Autor</t>
-  </si>
-  <si>
-    <t>Datum</t>
-  </si>
-  <si>
-    <t>Fabian Mauz</t>
-  </si>
-  <si>
-    <t>Messwert</t>
-  </si>
-  <si>
-    <t>Messung der Anzahl der Partikel in einer Mischung mit Alkohol</t>
+    <t>Test auf Aktivität A</t>
+  </si>
+  <si>
+    <t>Test auf Aktivität B</t>
+  </si>
+  <si>
+    <t>Test auf Aktivität C</t>
+  </si>
+  <si>
+    <t>0.01</t>
+  </si>
+  <si>
+    <t>.23</t>
+  </si>
+  <si>
+    <t>0.23</t>
+  </si>
+  <si>
+    <t>Autor:</t>
+  </si>
+  <si>
+    <t>Datum:</t>
+  </si>
+  <si>
+    <t>Dies ist ein Testtext für die eine genauere Definition von Probe 1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -46,16 +62,36 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -63,13 +99,293 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -374,140 +690,221 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:D20"/>
+  <dimension ref="B2:G19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.140625" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="1"/>
+    <col min="2" max="2" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.7109375" style="1" customWidth="1"/>
+    <col min="5" max="7" width="20.7109375" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B2" t="s">
+    <row r="2" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="22" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B3" s="22" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="23">
+        <v>44084</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="E5" s="2"/>
+    </row>
+    <row r="8" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="9" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D9" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C2" t="s">
+      <c r="E9" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="F9" s="3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B3" t="s">
+      <c r="G9" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="D10" s="7">
+        <v>1</v>
+      </c>
+      <c r="E10" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="F10" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="G10" s="10" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="D11" s="11">
         <v>2</v>
       </c>
-      <c r="C3" s="1">
-        <v>44075</v>
-      </c>
-    </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C4" s="1"/>
-    </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C5" s="1"/>
-    </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C6" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C7" s="1"/>
-    </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C8" s="1"/>
-    </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C10" t="s">
-        <v>0</v>
-      </c>
-      <c r="D10" t="s">
+      <c r="E11" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="F11" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="G11" s="14" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="D12" s="11">
+        <v>3</v>
+      </c>
+      <c r="E12" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="F12" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="G12" s="14" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="D13" s="11">
         <v>4</v>
       </c>
-    </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C11">
-        <v>1</v>
-      </c>
-      <c r="D11">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C12">
-        <v>2</v>
-      </c>
-      <c r="D12">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C13">
-        <v>3</v>
-      </c>
-      <c r="D13">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="14" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C14">
-        <v>4</v>
-      </c>
-      <c r="D14">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="15" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C15">
-        <v>5</v>
-      </c>
-      <c r="D15">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="16" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C16">
+      <c r="E13" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="F13" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="G13" s="14" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="D14" s="11">
+        <v>5</v>
+      </c>
+      <c r="E14" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="F14" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="D16">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="17" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C17">
+      <c r="G14" s="14" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="D15" s="11">
+        <v>6</v>
+      </c>
+      <c r="E15" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="F15" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="G15" s="14" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="D16" s="11">
         <v>7</v>
       </c>
-      <c r="D17">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="18" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C18">
+      <c r="E16" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="F16" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="G16" s="14" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D17" s="11">
         <v>8</v>
       </c>
-      <c r="D18">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="19" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C19">
+      <c r="E17" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="F17" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="G17" s="16" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D18" s="11">
         <v>9</v>
       </c>
-      <c r="D19">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="20" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C20">
+      <c r="E18" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="F18" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="G18" s="14" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="4:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D19" s="18">
         <v>10</v>
       </c>
-      <c r="D20">
-        <v>24</v>
+      <c r="E19" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="F19" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="G19" s="21" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="D7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="16384" width="11.42578125" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="7" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D7" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>